<commit_message>
versao final corrigir pequenos bugs
</commit_message>
<xml_diff>
--- a/daddos/planilha/Contatos.xlsx
+++ b/daddos/planilha/Contatos.xlsx
@@ -44,7 +44,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,25 +68,25 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFCCFFCC"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -128,15 +128,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -149,66 +149,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -395,7 +335,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -404,7 +344,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -412,12 +352,12 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">

</xml_diff>

<commit_message>
corrigido bug de celulas vazias
</commit_message>
<xml_diff>
--- a/daddos/planilha/Contatos.xlsx
+++ b/daddos/planilha/Contatos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">Nome</t>
   </si>
@@ -28,13 +28,16 @@
     <t xml:space="preserve">mensagem</t>
   </si>
   <si>
-    <t xml:space="preserve">vida</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oi, sou um robô programado por André</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paulo empresa</t>
+    <t xml:space="preserve">Andre MFprint </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ola</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nathaly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ola teste</t>
   </si>
 </sst>
 </file>
@@ -75,10 +78,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -128,15 +131,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -332,16 +335,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.38"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -349,7 +355,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -360,9 +366,12 @@
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>